<commit_message>
tratando de arreglar el error de que no encuentra los packahges
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/data.xlsx
+++ b/src/test/resources/datos/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara.alarcon\OneDrive - TSOFT\Escritorio\DesafioAutomatizacion\TrabajoPOM_alarcon\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{05C8B938-6AAC-49DB-890D-C960FC49F0E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5F7CDDBC-DBA5-4E89-8306-1D507F926053}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{05C8B938-6AAC-49DB-890D-C960FC49F0E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F4532274-E82A-4F25-8C2D-C4B6C87B5CD9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7200" xr2:uid="{13128920-B6FE-4053-B7E2-D49BE217C76D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -160,6 +160,27 @@
   </si>
   <si>
     <t>Ofertas</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>agosto 2023</t>
+  </si>
+  <si>
+    <t>Vuelo a Orlando</t>
+  </si>
+  <si>
+    <t>Despegar - Checkout</t>
+  </si>
+  <si>
+    <t>agosto 2024</t>
+  </si>
+  <si>
+    <t>Ingresa un destino</t>
+  </si>
+  <si>
+    <t>Ingresa una fecha de partida</t>
   </si>
 </sst>
 </file>
@@ -288,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -304,6 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +653,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,36 +748,6 @@
       <c r="I2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="2">
-        <v>3</v>
-      </c>
-      <c r="K2" s="2">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2">
-        <v>5</v>
-      </c>
-      <c r="M2" s="2">
-        <v>6</v>
-      </c>
-      <c r="N2" s="2">
-        <v>7</v>
-      </c>
-      <c r="O2" s="2">
-        <v>8</v>
-      </c>
-      <c r="P2" s="2">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>10</v>
-      </c>
-      <c r="R2" s="2">
-        <v>11</v>
-      </c>
-      <c r="S2" s="2">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -794,6 +786,12 @@
       <c r="L3" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="M3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -802,10 +800,40 @@
       <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="C4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -855,15 +883,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="44a8347a-f54a-44bc-8dc4-392ae4985b50" xsi:nil="true"/>
@@ -871,7 +890,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D9D086C79282EB40831F5A31AE1FD6DC" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b8e2e9e99a661fd1fd7652c191a46a12">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="44a8347a-f54a-44bc-8dc4-392ae4985b50" xmlns:ns4="e9945a31-c942-40c8-8c8e-a530049e7ab7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3e433a894c7e3a33bff5c9c6d5edb65" ns3:_="" ns4:_="">
     <xsd:import namespace="44a8347a-f54a-44bc-8dc4-392ae4985b50"/>
@@ -1080,32 +1099,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93C6BBF2-AF03-444C-A73E-E776970F6E96}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD5FC94C-3FC4-4D5B-9DC7-5D8F2FC5389A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e9945a31-c942-40c8-8c8e-a530049e7ab7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="44a8347a-f54a-44bc-8dc4-392ae4985b50"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD5FC94C-3FC4-4D5B-9DC7-5D8F2FC5389A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="44a8347a-f54a-44bc-8dc4-392ae4985b50"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e9945a31-c942-40c8-8c8e-a530049e7ab7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77A5678B-121E-4253-9A46-D2881CF6C5EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1122,4 +1142,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93C6BBF2-AF03-444C-A73E-E776970F6E96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>